<commit_message>
task sheet updated for the project
</commit_message>
<xml_diff>
--- a/CMPE202-TaskSheet.xlsx
+++ b/CMPE202-TaskSheet.xlsx
@@ -11,12 +11,11 @@
     <sheet name="Burndown" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Week #1 (10 hrs / week)</t>
   </si>
@@ -142,6 +141,9 @@
   </si>
   <si>
     <t>Updating Readme (project idea)</t>
+  </si>
+  <si>
+    <t>u</t>
   </si>
 </sst>
 </file>
@@ -554,7 +556,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -763,7 +764,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -820,11 +821,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="124299136"/>
-        <c:axId val="124301696"/>
+        <c:axId val="126782848"/>
+        <c:axId val="126789504"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="124299136"/>
+        <c:axId val="126782848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,7 +846,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="m&quot;/&quot;d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -859,13 +859,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124301696"/>
+        <c:crossAx val="126789504"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124301696"/>
+        <c:axId val="126789504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,7 +895,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -914,19 +913,18 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124299136"/>
+        <c:crossAx val="126782848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -944,7 +942,7 @@
     <xdr:ext cx="9763125" cy="4914900"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1253,7 +1251,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1480,7 +1478,7 @@
         <v>120</v>
       </c>
       <c r="E5" s="13">
-        <f t="shared" ref="E5:O5" si="0">SUM(E6:E14)</f>
+        <f t="shared" ref="E5:N5" si="0">SUM(E6:E14)</f>
         <v>40</v>
       </c>
       <c r="F5" s="14">
@@ -1497,7 +1495,7 @@
       </c>
       <c r="I5" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" s="14">
         <f t="shared" si="0"/>
@@ -1520,47 +1518,47 @@
         <v>0</v>
       </c>
       <c r="O5" s="14">
-        <f>SUM(O6:O14)</f>
+        <f t="shared" ref="O5:Y5" si="1">SUM(O6:O14)</f>
         <v>0</v>
       </c>
       <c r="P5" s="14">
-        <f>SUM(P6:P14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q5" s="14">
-        <f>SUM(Q6:Q14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R5" s="15">
-        <f>SUM(R6:R14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S5" s="13">
-        <f>SUM(S6:S14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T5" s="14">
-        <f>SUM(T6:T14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U5" s="14">
-        <f>SUM(U6:U14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V5" s="14">
-        <f>SUM(V6:V14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W5" s="14">
-        <f>SUM(W6:W14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X5" s="14">
-        <f>SUM(X6:X14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y5" s="15">
-        <f>SUM(Y6:Y14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z5" s="16" t="s">
@@ -1626,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="I7" s="21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" s="21"/>
       <c r="K7" s="22"/>
@@ -2103,7 +2101,9 @@
     <row r="24" spans="1:20" ht="13.2">
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
+      <c r="E24" s="34" t="s">
+        <v>42</v>
+      </c>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>

</xml_diff>